<commit_message>
update the database, include the excel and the sql
</commit_message>
<xml_diff>
--- a/document/危废仓储管理系统数据库设计.xlsx
+++ b/document/危废仓储管理系统数据库设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="仓储管理系统数据库说明" sheetId="4" r:id="rId1"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>外键waste表的主键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RFID标签编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,7 +150,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>外键，waste表的主键</t>
+    <t>外键fk_waste_id_production，waste表的主键waste_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_waste_id_receiving，waste表的主键waste_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -590,7 +590,7 @@
   <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -610,22 +610,22 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -638,16 +638,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -699,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -735,7 +737,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -762,10 +764,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -789,7 +791,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -797,7 +799,7 @@
     <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -848,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -892,10 +894,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -911,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>

</xml_diff>